<commit_message>
dispatch and code used in the current paper draft
</commit_message>
<xml_diff>
--- a/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
+++ b/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\sam_dev\sam-analyses\2023\mirletz_laws_pvsc\sam_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56047F2A-7A9B-4C19-BF3F-07E6C52BABD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4260B2FC-4B01-48AF-992F-3397F654D736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
+    <workbookView xWindow="38145" yWindow="2145" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E54FFCA-3A81-4895-A7A8-268220DEAC62}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
       <selection activeCell="Q20" sqref="Q20:R31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix nominal voltage versus high soc error, add new figure and plotting code for new figure
</commit_message>
<xml_diff>
--- a/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
+++ b/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\sam_dev\sam-analyses\2023\mirletz_laws_pvsc\sam_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4260B2FC-4B01-48AF-992F-3397F654D736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7568238-3B3B-44EC-92C7-5ADF4C86565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38145" yWindow="2145" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12360" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -475,7 +479,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,16 +506,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8130164</v>
+        <v>8119098</v>
       </c>
       <c r="C2">
-        <v>8882363</v>
+        <v>8839129</v>
       </c>
       <c r="D2">
-        <v>8430921</v>
+        <v>8433096</v>
       </c>
       <c r="E2">
-        <v>8698098</v>
+        <v>8694613</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -519,16 +523,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8031328</v>
+        <v>8045240</v>
       </c>
       <c r="C3">
-        <v>8514895</v>
+        <v>8487403</v>
       </c>
       <c r="D3">
-        <v>7387721</v>
+        <v>7398588</v>
       </c>
       <c r="E3">
-        <v>7618500</v>
+        <v>7618659</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -537,19 +541,19 @@
       </c>
       <c r="B4">
         <f>1-B3/B2</f>
-        <v>1.2156704342003444E-2</v>
+        <v>9.0968233170729551E-3</v>
       </c>
       <c r="C4">
         <f>1-C3/C2</f>
-        <v>4.1370522686361766E-2</v>
+        <v>3.9791929725202513E-2</v>
       </c>
       <c r="D4">
         <f>1-D3/D2</f>
-        <v>0.12373499882159966</v>
+        <v>0.12267238508846579</v>
       </c>
       <c r="E4">
         <f>1-E3/E2</f>
-        <v>0.12411885908850417</v>
+        <v>0.12374949868384022</v>
       </c>
     </row>
   </sheetData>
@@ -561,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E54FFCA-3A81-4895-A7A8-268220DEAC62}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20:R31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20:X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,10 +612,10 @@
       <c r="C3">
         <v>14576.3</v>
       </c>
-      <c r="E3">
-        <v>6663.46</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="1">
+        <v>6663.47</v>
+      </c>
+      <c r="F3" s="1">
         <v>14576.3</v>
       </c>
       <c r="H3">
@@ -620,10 +624,10 @@
       <c r="I3">
         <v>14576.3</v>
       </c>
-      <c r="K3">
-        <v>9950.83</v>
-      </c>
-      <c r="L3">
+      <c r="K3" s="3">
+        <v>9882.5</v>
+      </c>
+      <c r="L3" s="3">
         <v>14576.3</v>
       </c>
       <c r="N3">
@@ -661,10 +665,10 @@
       <c r="C4">
         <v>13895.1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>6492.63</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>13895.1</v>
       </c>
       <c r="H4">
@@ -673,10 +677,10 @@
       <c r="I4">
         <v>13895.1</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>9398.2999999999993</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>13895.1</v>
       </c>
       <c r="N4">
@@ -692,7 +696,7 @@
         <v>13895.1</v>
       </c>
       <c r="T4">
-        <v>3757.33</v>
+        <v>3757.32</v>
       </c>
       <c r="U4">
         <v>13895.1</v>
@@ -718,10 +722,10 @@
       <c r="C5">
         <v>14314.6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>6631.32</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>14314.6</v>
       </c>
       <c r="H5">
@@ -730,14 +734,14 @@
       <c r="I5">
         <v>14314.6</v>
       </c>
-      <c r="K5">
-        <v>11077.1</v>
-      </c>
-      <c r="L5">
+      <c r="K5" s="3">
+        <v>10699.5</v>
+      </c>
+      <c r="L5" s="3">
         <v>14314.6</v>
       </c>
       <c r="N5">
-        <v>5903.78</v>
+        <v>5903.77</v>
       </c>
       <c r="O5">
         <v>14314.6</v>
@@ -763,27 +767,27 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>6020.43</v>
+        <v>6162.55</v>
       </c>
       <c r="C6">
         <v>14556.4</v>
       </c>
-      <c r="E6">
-        <v>6417.1</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="1">
+        <v>6550.82</v>
+      </c>
+      <c r="F6" s="1">
         <v>14556.4</v>
       </c>
       <c r="H6">
-        <v>9373.76</v>
+        <v>9415.66</v>
       </c>
       <c r="I6">
         <v>14556.4</v>
       </c>
-      <c r="K6">
-        <v>12871.7</v>
-      </c>
-      <c r="L6">
+      <c r="K6" s="3">
+        <v>12516.2</v>
+      </c>
+      <c r="L6" s="3">
         <v>14556.4</v>
       </c>
       <c r="N6">
@@ -805,7 +809,7 @@
         <v>14556.4</v>
       </c>
       <c r="W6">
-        <v>15709.4</v>
+        <v>15662.2</v>
       </c>
       <c r="X6">
         <v>14556.4</v>
@@ -813,15 +817,15 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B7">
-        <v>7226.33</v>
+        <v>7087.48</v>
       </c>
       <c r="C7">
         <v>14459.1</v>
       </c>
-      <c r="E7">
-        <v>8438.49</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="1">
+        <v>8229.9500000000007</v>
+      </c>
+      <c r="F7" s="1">
         <v>14459.1</v>
       </c>
       <c r="H7">
@@ -830,10 +834,10 @@
       <c r="I7">
         <v>14459.1</v>
       </c>
-      <c r="K7">
-        <v>12012.7</v>
-      </c>
-      <c r="L7">
+      <c r="K7" s="3">
+        <v>11457.5</v>
+      </c>
+      <c r="L7" s="3">
         <v>14459.1</v>
       </c>
       <c r="N7">
@@ -843,7 +847,7 @@
         <v>14459.1</v>
       </c>
       <c r="Q7">
-        <v>11428.3</v>
+        <v>11436.6</v>
       </c>
       <c r="R7">
         <v>14459.1</v>
@@ -863,15 +867,15 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B8">
-        <v>10221.5</v>
+        <v>9921.1200000000008</v>
       </c>
       <c r="C8">
         <v>14896.1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>12499.4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>14896.1</v>
       </c>
       <c r="H8">
@@ -880,10 +884,10 @@
       <c r="I8">
         <v>14896.1</v>
       </c>
-      <c r="K8">
-        <v>18532.7</v>
-      </c>
-      <c r="L8">
+      <c r="K8" s="3">
+        <v>18086.8</v>
+      </c>
+      <c r="L8" s="3">
         <v>14896.1</v>
       </c>
       <c r="N8">
@@ -899,7 +903,7 @@
         <v>14896.1</v>
       </c>
       <c r="T8">
-        <v>7056.09</v>
+        <v>7376</v>
       </c>
       <c r="U8">
         <v>14896.1</v>
@@ -913,15 +917,15 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B9">
-        <v>6744.8</v>
+        <v>6871.79</v>
       </c>
       <c r="C9">
         <v>14901.8</v>
       </c>
-      <c r="E9">
-        <v>7269</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="1">
+        <v>7454.73</v>
+      </c>
+      <c r="F9" s="1">
         <v>14901.8</v>
       </c>
       <c r="H9">
@@ -930,10 +934,10 @@
       <c r="I9">
         <v>14901.8</v>
       </c>
-      <c r="K9">
-        <v>16123.1</v>
-      </c>
-      <c r="L9">
+      <c r="K9" s="3">
+        <v>15591.9</v>
+      </c>
+      <c r="L9" s="3">
         <v>14901.8</v>
       </c>
       <c r="N9">
@@ -943,7 +947,7 @@
         <v>14901.8</v>
       </c>
       <c r="Q9">
-        <v>12809.7</v>
+        <v>11527.4</v>
       </c>
       <c r="R9">
         <v>14901.8</v>
@@ -963,15 +967,15 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B10">
-        <v>7828.11</v>
+        <v>8014.91</v>
       </c>
       <c r="C10">
         <v>15058.7</v>
       </c>
-      <c r="E10">
-        <v>8954.85</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="1">
+        <v>9125.98</v>
+      </c>
+      <c r="F10" s="1">
         <v>15058.7</v>
       </c>
       <c r="H10">
@@ -980,10 +984,10 @@
       <c r="I10">
         <v>15058.7</v>
       </c>
-      <c r="K10">
-        <v>18871.7</v>
-      </c>
-      <c r="L10">
+      <c r="K10" s="3">
+        <v>18331.8</v>
+      </c>
+      <c r="L10" s="3">
         <v>15058.7</v>
       </c>
       <c r="N10">
@@ -1013,15 +1017,15 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>7177.89</v>
+        <v>7351.64</v>
       </c>
       <c r="C11">
         <v>15203.5</v>
       </c>
-      <c r="E11">
-        <v>9128.84</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="1">
+        <v>8900.27</v>
+      </c>
+      <c r="F11" s="1">
         <v>15203.5</v>
       </c>
       <c r="H11">
@@ -1030,14 +1034,14 @@
       <c r="I11">
         <v>15203.5</v>
       </c>
-      <c r="K11">
-        <v>16017.9</v>
-      </c>
-      <c r="L11">
+      <c r="K11" s="3">
+        <v>15554.3</v>
+      </c>
+      <c r="L11" s="3">
         <v>15203.5</v>
       </c>
       <c r="N11">
-        <v>7042.57</v>
+        <v>7042.58</v>
       </c>
       <c r="O11">
         <v>15203.5</v>
@@ -1049,7 +1053,7 @@
         <v>15203.5</v>
       </c>
       <c r="T11">
-        <v>6129.12</v>
+        <v>6412.75</v>
       </c>
       <c r="U11">
         <v>15203.5</v>
@@ -1063,27 +1067,27 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B12">
-        <v>7963.2</v>
+        <v>8143.59</v>
       </c>
       <c r="C12">
         <v>14877.2</v>
       </c>
-      <c r="E12">
-        <v>8426.7800000000007</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="1">
+        <v>8836.15</v>
+      </c>
+      <c r="F12" s="1">
         <v>14877.2</v>
       </c>
       <c r="H12">
-        <v>9917.8700000000008</v>
+        <v>11312.5</v>
       </c>
       <c r="I12">
         <v>14877.2</v>
       </c>
-      <c r="K12">
-        <v>18877</v>
-      </c>
-      <c r="L12">
+      <c r="K12" s="3">
+        <v>18336.599999999999</v>
+      </c>
+      <c r="L12" s="3">
         <v>14877.2</v>
       </c>
       <c r="N12">
@@ -1113,27 +1117,27 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B13">
-        <v>8860.2000000000007</v>
+        <v>9282.35</v>
       </c>
       <c r="C13">
         <v>14976.4</v>
       </c>
-      <c r="E13">
-        <v>10920.3</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="1">
+        <v>10476</v>
+      </c>
+      <c r="F13" s="1">
         <v>14976.4</v>
       </c>
       <c r="H13">
-        <v>11447.3</v>
+        <v>10257.700000000001</v>
       </c>
       <c r="I13">
         <v>14976.4</v>
       </c>
-      <c r="K13">
-        <v>18103.3</v>
-      </c>
-      <c r="L13">
+      <c r="K13" s="3">
+        <v>17541.599999999999</v>
+      </c>
+      <c r="L13" s="3">
         <v>14976.4</v>
       </c>
       <c r="N13">
@@ -1163,27 +1167,27 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B14">
-        <v>6511.04</v>
+        <v>6540.57</v>
       </c>
       <c r="C14">
         <v>14456.5</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>6584.05</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>14456.5</v>
       </c>
       <c r="H14">
-        <v>9343.99</v>
+        <v>9331.69</v>
       </c>
       <c r="I14">
         <v>14456.5</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="3">
         <v>10518.1</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="3">
         <v>14456.5</v>
       </c>
       <c r="N14">
@@ -1217,7 +1221,7 @@
       </c>
       <c r="B16">
         <f>SUM(B3:B14)</f>
-        <v>89577.409999999989</v>
+        <v>90399.91</v>
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
@@ -1225,7 +1229,7 @@
       </c>
       <c r="E16">
         <f>SUM(E3:E14)</f>
-        <v>98426.22</v>
+        <v>98444.77</v>
       </c>
       <c r="F16">
         <f>SUM(F3:F14)</f>
@@ -1233,7 +1237,7 @@
       </c>
       <c r="H16">
         <f>SUM(H3:H14)</f>
-        <v>119866.36</v>
+        <v>120100.98999999999</v>
       </c>
       <c r="I16">
         <f>SUM(I3:I14)</f>
@@ -1241,7 +1245,7 @@
       </c>
       <c r="K16">
         <f>SUM(K3:K14)</f>
-        <v>172354.42999999996</v>
+        <v>167915.1</v>
       </c>
       <c r="L16">
         <f>SUM(L3:L14)</f>
@@ -1257,7 +1261,7 @@
       </c>
       <c r="Q16">
         <f>SUM(Q3:Q14)</f>
-        <v>180158.7</v>
+        <v>178884.69999999998</v>
       </c>
       <c r="R16">
         <f>SUM(R3:R14)</f>
@@ -1265,7 +1269,7 @@
       </c>
       <c r="T16">
         <f>SUM(T3:T14)</f>
-        <v>64995.100000000006</v>
+        <v>65598.63</v>
       </c>
       <c r="U16">
         <f>SUM(U3:U14)</f>
@@ -1273,7 +1277,7 @@
       </c>
       <c r="W16">
         <f>SUM(W3:W14)</f>
-        <v>189845.3</v>
+        <v>189798.1</v>
       </c>
       <c r="X16">
         <f>SUM(X3:X14)</f>
@@ -1286,19 +1290,19 @@
       </c>
       <c r="C17">
         <f>C16-B16</f>
-        <v>86594.290000000023</v>
+        <v>85771.790000000008</v>
       </c>
       <c r="F17">
         <f>F16-E16</f>
-        <v>77745.48000000001</v>
+        <v>77726.930000000008</v>
       </c>
       <c r="I17">
         <f>I16-H16</f>
-        <v>56305.340000000011</v>
+        <v>56070.710000000021</v>
       </c>
       <c r="L17">
         <f>L16-K16</f>
-        <v>3817.2700000000477</v>
+        <v>8256.6000000000058</v>
       </c>
       <c r="O17">
         <f>O16-N16</f>
@@ -1306,15 +1310,15 @@
       </c>
       <c r="R17">
         <f>R16-Q16</f>
-        <v>-3987</v>
+        <v>-2712.9999999999709</v>
       </c>
       <c r="U17">
         <f>U16-T16</f>
-        <v>111176.6</v>
+        <v>110573.07</v>
       </c>
       <c r="X17">
         <f>X16-W16</f>
-        <v>-13673.599999999977</v>
+        <v>-13626.399999999994</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
@@ -1323,35 +1327,35 @@
       </c>
       <c r="F18">
         <f>C17-F17</f>
-        <v>8848.8100000000122</v>
+        <v>8044.8600000000006</v>
       </c>
       <c r="G18">
         <f>1-F17/C17</f>
-        <v>0.10218699177509294</v>
+        <v>9.3793775319367834E-2</v>
       </c>
       <c r="L18">
         <f>I17-L17</f>
-        <v>52488.069999999963</v>
+        <v>47814.110000000015</v>
       </c>
       <c r="M18">
         <f>1-L17/I17</f>
-        <v>0.93220412131424757</v>
+        <v>0.85274664793793398</v>
       </c>
       <c r="R18">
         <f>O17-R17</f>
-        <v>98873.530000000013</v>
+        <v>97599.529999999984</v>
       </c>
       <c r="S18">
         <f>1-R17/O17</f>
-        <v>1.0420186089637802</v>
+        <v>1.0285920456781377</v>
       </c>
       <c r="X18">
         <f>U17-X17</f>
-        <v>124850.19999999998</v>
+        <v>124199.47</v>
       </c>
       <c r="Y18">
         <f>1-X17/U17</f>
-        <v>1.1229899097471947</v>
+        <v>1.1232343463015</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
@@ -1361,49 +1365,49 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>24821.9</v>
+        <v>24850.1</v>
       </c>
       <c r="C20">
         <v>136681</v>
       </c>
-      <c r="E20">
-        <v>25563.4</v>
-      </c>
-      <c r="F20">
+      <c r="E20" s="2">
+        <v>25530</v>
+      </c>
+      <c r="F20" s="2">
         <v>136681</v>
       </c>
       <c r="H20">
-        <v>13303</v>
+        <v>13936.5</v>
       </c>
       <c r="I20">
         <v>136681</v>
       </c>
-      <c r="K20">
-        <v>12783.2</v>
-      </c>
-      <c r="L20">
+      <c r="K20" s="4">
+        <v>13577.5</v>
+      </c>
+      <c r="L20" s="4">
         <v>136681</v>
       </c>
       <c r="N20">
-        <v>22641.8</v>
+        <v>22626.3</v>
       </c>
       <c r="O20">
         <v>136681</v>
       </c>
       <c r="Q20">
-        <v>23126.2</v>
+        <v>23260.400000000001</v>
       </c>
       <c r="R20">
         <v>136681</v>
       </c>
       <c r="T20">
-        <v>19959.599999999999</v>
+        <v>19961.400000000001</v>
       </c>
       <c r="U20">
         <v>136681</v>
       </c>
       <c r="W20">
-        <v>21048.7</v>
+        <v>21047.7</v>
       </c>
       <c r="X20">
         <v>136681</v>
@@ -1411,49 +1415,49 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>16353.4</v>
+        <v>16698.2</v>
       </c>
       <c r="C21">
         <v>119047</v>
       </c>
-      <c r="E21">
-        <v>17935.5</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="2">
+        <v>17915.599999999999</v>
+      </c>
+      <c r="F21" s="2">
         <v>119047</v>
       </c>
       <c r="H21">
-        <v>7095.31</v>
+        <v>7732.89</v>
       </c>
       <c r="I21">
         <v>119047</v>
       </c>
-      <c r="K21">
-        <v>7361.14</v>
-      </c>
-      <c r="L21">
+      <c r="K21" s="4">
+        <v>8047.9</v>
+      </c>
+      <c r="L21" s="4">
         <v>119047</v>
       </c>
       <c r="N21">
-        <v>14163.1</v>
+        <v>14141.4</v>
       </c>
       <c r="O21">
         <v>119047</v>
       </c>
       <c r="Q21">
-        <v>16137.9</v>
+        <v>16152.8</v>
       </c>
       <c r="R21">
         <v>119047</v>
       </c>
       <c r="T21">
-        <v>9343.82</v>
+        <v>9345.9</v>
       </c>
       <c r="U21">
         <v>119047</v>
       </c>
       <c r="W21">
-        <v>13592.8</v>
+        <v>13590.9</v>
       </c>
       <c r="X21">
         <v>119047</v>
@@ -1461,49 +1465,49 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22">
-        <v>25348.9</v>
+        <v>25580.400000000001</v>
       </c>
       <c r="C22">
         <v>135863</v>
       </c>
-      <c r="E22">
-        <v>26686.1</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="2">
+        <v>26628.400000000001</v>
+      </c>
+      <c r="F22" s="2">
         <v>135863</v>
       </c>
       <c r="H22">
-        <v>14695.8</v>
+        <v>15528.9</v>
       </c>
       <c r="I22">
         <v>135863</v>
       </c>
-      <c r="K22">
-        <v>13569.7</v>
-      </c>
-      <c r="L22">
+      <c r="K22" s="4">
+        <v>14356.9</v>
+      </c>
+      <c r="L22" s="4">
         <v>135863</v>
       </c>
       <c r="N22">
-        <v>23255.4</v>
+        <v>23248.799999999999</v>
       </c>
       <c r="O22">
         <v>135863</v>
       </c>
       <c r="Q22">
-        <v>25964.2</v>
+        <v>26074.799999999999</v>
       </c>
       <c r="R22">
         <v>135863</v>
       </c>
       <c r="T22">
-        <v>19335.7</v>
+        <v>19335.3</v>
       </c>
       <c r="U22">
         <v>135863</v>
       </c>
       <c r="W22">
-        <v>21764.400000000001</v>
+        <v>21761</v>
       </c>
       <c r="X22">
         <v>135863</v>
@@ -1511,49 +1515,49 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>17563.599999999999</v>
+        <v>17723.8</v>
       </c>
       <c r="C23">
         <v>132398</v>
       </c>
-      <c r="E23">
-        <v>18559.900000000001</v>
-      </c>
-      <c r="F23">
+      <c r="E23" s="2">
+        <v>18477.5</v>
+      </c>
+      <c r="F23" s="2">
         <v>132398</v>
       </c>
       <c r="H23">
-        <v>7470.82</v>
+        <v>8274.39</v>
       </c>
       <c r="I23">
         <v>132398</v>
       </c>
-      <c r="K23">
-        <v>7447.12</v>
-      </c>
-      <c r="L23">
+      <c r="K23" s="4">
+        <v>8076.78</v>
+      </c>
+      <c r="L23" s="4">
         <v>132398</v>
       </c>
       <c r="N23">
-        <v>15048.4</v>
+        <v>15011.6</v>
       </c>
       <c r="O23">
         <v>132398</v>
       </c>
       <c r="Q23">
-        <v>17400.900000000001</v>
+        <v>17479.099999999999</v>
       </c>
       <c r="R23">
         <v>132398</v>
       </c>
       <c r="T23">
-        <v>11765.4</v>
+        <v>11767.7</v>
       </c>
       <c r="U23">
         <v>132398</v>
       </c>
       <c r="W23">
-        <v>14765.6</v>
+        <v>14763</v>
       </c>
       <c r="X23">
         <v>132398</v>
@@ -1561,49 +1565,49 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B24">
-        <v>28206.400000000001</v>
+        <v>28336.6</v>
       </c>
       <c r="C24">
         <v>139577</v>
       </c>
-      <c r="E24">
-        <v>28275.7</v>
-      </c>
-      <c r="F24">
+      <c r="E24" s="2">
+        <v>28433.1</v>
+      </c>
+      <c r="F24" s="2">
         <v>139577</v>
       </c>
       <c r="H24">
-        <v>15942.9</v>
+        <v>16828.900000000001</v>
       </c>
       <c r="I24">
         <v>139577</v>
       </c>
-      <c r="K24">
-        <v>15874.7</v>
-      </c>
-      <c r="L24">
+      <c r="K24" s="4">
+        <v>16958.599999999999</v>
+      </c>
+      <c r="L24" s="4">
         <v>139577</v>
       </c>
       <c r="N24">
-        <v>25968.3</v>
+        <v>25950.6</v>
       </c>
       <c r="O24">
         <v>139577</v>
       </c>
       <c r="Q24">
-        <v>28480</v>
+        <v>28625.4</v>
       </c>
       <c r="R24">
         <v>139577</v>
       </c>
       <c r="T24">
-        <v>23065.3</v>
+        <v>23066.1</v>
       </c>
       <c r="U24">
         <v>139577</v>
       </c>
       <c r="W24">
-        <v>25095.8</v>
+        <v>25093.7</v>
       </c>
       <c r="X24">
         <v>139577</v>
@@ -1611,49 +1615,49 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B25">
-        <v>28573.1</v>
+        <v>28673.1</v>
       </c>
       <c r="C25">
         <v>140124</v>
       </c>
-      <c r="E25">
-        <v>29340</v>
-      </c>
-      <c r="F25">
+      <c r="E25" s="2">
+        <v>29350.400000000001</v>
+      </c>
+      <c r="F25" s="2">
         <v>140124</v>
       </c>
       <c r="H25">
-        <v>17573.099999999999</v>
+        <v>18325</v>
       </c>
       <c r="I25">
         <v>140124</v>
       </c>
-      <c r="K25">
-        <v>17853.3</v>
-      </c>
-      <c r="L25">
+      <c r="K25" s="4">
+        <v>18367.400000000001</v>
+      </c>
+      <c r="L25" s="4">
         <v>140124</v>
       </c>
       <c r="N25">
-        <v>26266.6</v>
+        <v>26243.7</v>
       </c>
       <c r="O25">
         <v>140124</v>
       </c>
       <c r="Q25">
-        <v>28653.9</v>
+        <v>28632.9</v>
       </c>
       <c r="R25">
         <v>140124</v>
       </c>
       <c r="T25">
-        <v>29046.2</v>
+        <v>29055.5</v>
       </c>
       <c r="U25">
         <v>140124</v>
       </c>
       <c r="W25">
-        <v>25184.1</v>
+        <v>25187.200000000001</v>
       </c>
       <c r="X25">
         <v>140124</v>
@@ -1661,49 +1665,49 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>28327.1</v>
+        <v>28617.5</v>
       </c>
       <c r="C26">
         <v>142832</v>
       </c>
-      <c r="E26">
-        <v>28858.2</v>
-      </c>
-      <c r="F26">
+      <c r="E26" s="2">
+        <v>28917.3</v>
+      </c>
+      <c r="F26" s="2">
         <v>142832</v>
       </c>
       <c r="H26">
-        <v>19378.8</v>
+        <v>19766</v>
       </c>
       <c r="I26">
         <v>142832</v>
       </c>
-      <c r="K26">
-        <v>18284.8</v>
-      </c>
-      <c r="L26">
+      <c r="K26" s="4">
+        <v>18874.7</v>
+      </c>
+      <c r="L26" s="4">
         <v>142832</v>
       </c>
       <c r="N26">
-        <v>24785.7</v>
+        <v>24778.5</v>
       </c>
       <c r="O26">
         <v>142832</v>
       </c>
       <c r="Q26">
-        <v>28257.7</v>
+        <v>28250.9</v>
       </c>
       <c r="R26">
         <v>142832</v>
       </c>
       <c r="T26">
-        <v>24066.9</v>
+        <v>24069.3</v>
       </c>
       <c r="U26">
         <v>142832</v>
       </c>
       <c r="W26">
-        <v>26360.1</v>
+        <v>26357.1</v>
       </c>
       <c r="X26">
         <v>142832</v>
@@ -1711,49 +1715,49 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>31394.3</v>
+        <v>31599.200000000001</v>
       </c>
       <c r="C27">
         <v>147121</v>
       </c>
-      <c r="E27">
-        <v>32062.799999999999</v>
-      </c>
-      <c r="F27">
+      <c r="E27" s="2">
+        <v>31931.3</v>
+      </c>
+      <c r="F27" s="2">
         <v>147121</v>
       </c>
       <c r="H27">
-        <v>20399</v>
+        <v>20738.599999999999</v>
       </c>
       <c r="I27">
         <v>147121</v>
       </c>
-      <c r="K27">
-        <v>19597.099999999999</v>
-      </c>
-      <c r="L27">
+      <c r="K27" s="4">
+        <v>20419.3</v>
+      </c>
+      <c r="L27" s="4">
         <v>147121</v>
       </c>
       <c r="N27">
-        <v>28748.9</v>
+        <v>28747.200000000001</v>
       </c>
       <c r="O27">
         <v>147121</v>
       </c>
       <c r="Q27">
-        <v>31147.5</v>
+        <v>31078.2</v>
       </c>
       <c r="R27">
         <v>147121</v>
       </c>
       <c r="T27">
-        <v>28839.599999999999</v>
+        <v>28837</v>
       </c>
       <c r="U27">
         <v>147121</v>
       </c>
       <c r="W27">
-        <v>28265.5</v>
+        <v>28273.4</v>
       </c>
       <c r="X27">
         <v>147121</v>
@@ -1761,49 +1765,49 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>28676.400000000001</v>
+        <v>28788.1</v>
       </c>
       <c r="C28">
         <v>140368</v>
       </c>
-      <c r="E28">
-        <v>28554.2</v>
-      </c>
-      <c r="F28">
+      <c r="E28" s="2">
+        <v>28739.9</v>
+      </c>
+      <c r="F28" s="2">
         <v>140368</v>
       </c>
       <c r="H28">
-        <v>17965.5</v>
+        <v>18376.8</v>
       </c>
       <c r="I28">
         <v>140368</v>
       </c>
-      <c r="K28">
-        <v>17508.8</v>
-      </c>
-      <c r="L28">
+      <c r="K28" s="4">
+        <v>18131.8</v>
+      </c>
+      <c r="L28" s="4">
         <v>140368</v>
       </c>
       <c r="N28">
-        <v>26928.799999999999</v>
+        <v>26907.1</v>
       </c>
       <c r="O28">
         <v>140368</v>
       </c>
       <c r="Q28">
-        <v>28200.5</v>
+        <v>28152.2</v>
       </c>
       <c r="R28">
         <v>140368</v>
       </c>
       <c r="T28">
-        <v>24801.8</v>
+        <v>24798.799999999999</v>
       </c>
       <c r="U28">
         <v>140368</v>
       </c>
       <c r="W28">
-        <v>24845.3</v>
+        <v>24842.2</v>
       </c>
       <c r="X28">
         <v>140368</v>
@@ -1811,49 +1815,49 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29">
-        <v>32601</v>
+        <v>32493.8</v>
       </c>
       <c r="C29">
         <v>142469</v>
       </c>
-      <c r="E29">
-        <v>31662.3</v>
-      </c>
-      <c r="F29">
+      <c r="E29" s="2">
+        <v>31415.7</v>
+      </c>
+      <c r="F29" s="2">
         <v>142469</v>
       </c>
       <c r="H29">
-        <v>22230.3</v>
+        <v>22316.9</v>
       </c>
       <c r="I29">
         <v>142469</v>
       </c>
-      <c r="K29">
-        <v>19438.7</v>
-      </c>
-      <c r="L29">
+      <c r="K29" s="4">
+        <v>20289.7</v>
+      </c>
+      <c r="L29" s="4">
         <v>142469</v>
       </c>
       <c r="N29">
-        <v>30300.3</v>
+        <v>30286.2</v>
       </c>
       <c r="O29">
         <v>142469</v>
       </c>
       <c r="Q29">
-        <v>30875.1</v>
+        <v>30938.3</v>
       </c>
       <c r="R29">
         <v>142469</v>
       </c>
       <c r="T29">
-        <v>31696.1</v>
+        <v>31694.5</v>
       </c>
       <c r="U29">
         <v>142469</v>
       </c>
       <c r="W29">
-        <v>28443.1</v>
+        <v>28450.2</v>
       </c>
       <c r="X29">
         <v>142469</v>
@@ -1861,49 +1865,49 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30">
-        <v>26087.5</v>
+        <v>26037</v>
       </c>
       <c r="C30">
         <v>137239</v>
       </c>
-      <c r="E30">
-        <v>26044.5</v>
-      </c>
-      <c r="F30">
+      <c r="E30" s="2">
+        <v>26037.5</v>
+      </c>
+      <c r="F30" s="2">
         <v>137239</v>
       </c>
       <c r="H30">
-        <v>15541.9</v>
+        <v>16073.6</v>
       </c>
       <c r="I30">
         <v>137239</v>
       </c>
-      <c r="K30">
-        <v>13080.7</v>
-      </c>
-      <c r="L30">
+      <c r="K30" s="4">
+        <v>13720.5</v>
+      </c>
+      <c r="L30" s="4">
         <v>137239</v>
       </c>
       <c r="N30">
-        <v>24237.5</v>
+        <v>24212.7</v>
       </c>
       <c r="O30">
         <v>137239</v>
       </c>
       <c r="Q30">
-        <v>23911.200000000001</v>
+        <v>24002.1</v>
       </c>
       <c r="R30">
         <v>137239</v>
       </c>
       <c r="T30">
-        <v>24750.799999999999</v>
+        <v>24749.200000000001</v>
       </c>
       <c r="U30">
         <v>137239</v>
       </c>
       <c r="W30">
-        <v>22467.599999999999</v>
+        <v>22464.9</v>
       </c>
       <c r="X30">
         <v>137239</v>
@@ -1911,49 +1915,49 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B31">
-        <v>24991.8</v>
+        <v>24918.7</v>
       </c>
       <c r="C31">
         <v>135534</v>
       </c>
-      <c r="E31">
-        <v>25102.6</v>
-      </c>
-      <c r="F31">
+      <c r="E31" s="2">
+        <v>24975</v>
+      </c>
+      <c r="F31" s="2">
         <v>135534</v>
       </c>
       <c r="H31">
-        <v>13666.1</v>
+        <v>14582</v>
       </c>
       <c r="I31">
         <v>135534</v>
       </c>
-      <c r="K31">
-        <v>12304.7</v>
-      </c>
-      <c r="L31">
+      <c r="K31" s="4">
+        <v>13015.7</v>
+      </c>
+      <c r="L31" s="4">
         <v>135534</v>
       </c>
       <c r="N31">
-        <v>23229.200000000001</v>
+        <v>23179.1</v>
       </c>
       <c r="O31">
         <v>135534</v>
       </c>
       <c r="Q31">
-        <v>22909.599999999999</v>
+        <v>22985.599999999999</v>
       </c>
       <c r="R31">
         <v>135534</v>
       </c>
       <c r="T31">
-        <v>19929.7</v>
+        <v>19926</v>
       </c>
       <c r="U31">
         <v>135534</v>
       </c>
       <c r="W31">
-        <v>19830.3</v>
+        <v>19826.099999999999</v>
       </c>
       <c r="X31">
         <v>135534</v>
@@ -1962,7 +1966,7 @@
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B33">
         <f>SUM(B20:B31)</f>
-        <v>312945.39999999997</v>
+        <v>314316.50000000006</v>
       </c>
       <c r="C33">
         <f>SUM(C20:C31)</f>
@@ -1970,7 +1974,7 @@
       </c>
       <c r="E33">
         <f>SUM(E20:E31)</f>
-        <v>318645.19999999995</v>
+        <v>318351.69999999995</v>
       </c>
       <c r="F33">
         <f>SUM(F20:F31)</f>
@@ -1978,7 +1982,7 @@
       </c>
       <c r="H33">
         <f>SUM(H20:H31)</f>
-        <v>185262.52999999997</v>
+        <v>192480.47999999998</v>
       </c>
       <c r="I33">
         <f>SUM(I20:I31)</f>
@@ -1986,7 +1990,7 @@
       </c>
       <c r="K33">
         <f>SUM(K20:K31)</f>
-        <v>175103.96000000002</v>
+        <v>183836.78000000003</v>
       </c>
       <c r="L33">
         <f>SUM(L20:L31)</f>
@@ -1994,7 +1998,7 @@
       </c>
       <c r="N33">
         <f>SUM(N20:N31)</f>
-        <v>285574</v>
+        <v>285333.2</v>
       </c>
       <c r="O33">
         <f>SUM(O20:O31)</f>
@@ -2002,7 +2006,7 @@
       </c>
       <c r="Q33">
         <f>SUM(Q20:Q31)</f>
-        <v>305064.7</v>
+        <v>305632.69999999995</v>
       </c>
       <c r="R33">
         <f>SUM(R20:R31)</f>
@@ -2010,7 +2014,7 @@
       </c>
       <c r="T33">
         <f>SUM(T20:T31)</f>
-        <v>266600.92</v>
+        <v>266606.69999999995</v>
       </c>
       <c r="U33">
         <f>SUM(U20:U31)</f>
@@ -2018,7 +2022,7 @@
       </c>
       <c r="W33">
         <f>SUM(W20:W31)</f>
-        <v>271663.3</v>
+        <v>271657.40000000002</v>
       </c>
       <c r="X33">
         <f>SUM(X20:X31)</f>
@@ -2031,51 +2035,51 @@
       </c>
       <c r="C34">
         <f>C33-B33</f>
-        <v>1336307.6000000001</v>
+        <v>1334936.5</v>
       </c>
       <c r="F34">
         <f>F33-E33</f>
-        <v>1330607.8</v>
+        <v>1330901.3</v>
       </c>
       <c r="G34">
         <f>1-F34/C34</f>
-        <v>4.265335316509522E-3</v>
+        <v>3.0227655023290501E-3</v>
       </c>
       <c r="I34">
         <f>I33-H33</f>
-        <v>1463990.47</v>
+        <v>1456772.52</v>
       </c>
       <c r="L34">
         <f>L33-K33</f>
-        <v>1474149.04</v>
+        <v>1465416.22</v>
       </c>
       <c r="M34">
         <f>1-L34/I34</f>
-        <v>-6.9389591040165399E-3</v>
+        <v>-5.9334589864448173E-3</v>
       </c>
       <c r="O34">
         <f>O33-N33</f>
-        <v>1363679</v>
+        <v>1363919.8</v>
       </c>
       <c r="R34">
         <f>R33-Q33</f>
-        <v>1344188.3</v>
+        <v>1343620.3</v>
       </c>
       <c r="S34">
         <f>1-R34/O34</f>
-        <v>1.4292733113877909E-2</v>
+        <v>1.4883206475923338E-2</v>
       </c>
       <c r="U34">
         <f>U33-T33</f>
-        <v>1382652.08</v>
+        <v>1382646.3</v>
       </c>
       <c r="X34">
         <f>X33-W33</f>
-        <v>1377589.7</v>
+        <v>1377595.6</v>
       </c>
       <c r="Y34">
         <f>1-X34/U34</f>
-        <v>3.6613549230694042E-3</v>
+        <v>3.6529226599745224E-3</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
@@ -2084,19 +2088,19 @@
       </c>
       <c r="F35">
         <f>C34-F34</f>
-        <v>5699.8000000000466</v>
+        <v>4035.1999999999534</v>
       </c>
       <c r="L35">
         <f>I34-L34</f>
-        <v>-10158.570000000065</v>
+        <v>-8643.6999999999534</v>
       </c>
       <c r="R35">
         <f>O34-R34</f>
-        <v>19490.699999999953</v>
+        <v>20299.5</v>
       </c>
       <c r="X35">
         <f>U34-X34</f>
-        <v>5062.3800000001211</v>
+        <v>5050.6999999999534</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
@@ -2105,35 +2109,35 @@
       </c>
       <c r="C36">
         <f>C17+C34</f>
-        <v>1422901.8900000001</v>
+        <v>1420708.29</v>
       </c>
       <c r="F36">
         <f>F17+F34</f>
-        <v>1408353.28</v>
+        <v>1408628.23</v>
       </c>
       <c r="I36">
         <f>I17+I34</f>
-        <v>1520295.81</v>
+        <v>1512843.23</v>
       </c>
       <c r="L36">
         <f>L17+L34</f>
-        <v>1477966.31</v>
+        <v>1473672.82</v>
       </c>
       <c r="O36">
         <f>O17+O34</f>
-        <v>1458565.53</v>
+        <v>1458806.33</v>
       </c>
       <c r="R36">
         <f>R17+R34</f>
-        <v>1340201.3</v>
+        <v>1340907.3</v>
       </c>
       <c r="U36">
         <f>U17+U34</f>
-        <v>1493828.6800000002</v>
+        <v>1493219.37</v>
       </c>
       <c r="X36">
         <f>X17+X34</f>
-        <v>1363916.1</v>
+        <v>1363969.2000000002</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
@@ -2142,19 +2146,19 @@
       </c>
       <c r="F37">
         <f>C36-F36</f>
-        <v>14548.610000000102</v>
+        <v>12080.060000000056</v>
       </c>
       <c r="L37">
         <f>I36-L36</f>
-        <v>42329.5</v>
+        <v>39170.409999999916</v>
       </c>
       <c r="R37">
         <f>O36-R36</f>
-        <v>118364.22999999998</v>
+        <v>117899.03000000003</v>
       </c>
       <c r="X37">
         <f>U36-X36</f>
-        <v>129912.58000000007</v>
+        <v>129250.16999999993</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
@@ -2163,19 +2167,19 @@
       </c>
       <c r="F39">
         <f>F18/F37</f>
-        <v>0.60822374096219156</v>
+        <v>0.66596192403017562</v>
       </c>
       <c r="L39">
         <f>L18/L37</f>
-        <v>1.2399879516649137</v>
+        <v>1.2206691224319612</v>
       </c>
       <c r="R39">
         <f>R18/R37</f>
-        <v>0.83533285351495146</v>
+        <v>0.82782301092723121</v>
       </c>
       <c r="X39">
         <f>X18/X37</f>
-        <v>0.96103241117988658</v>
+        <v>0.96092306880524858</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
@@ -2184,19 +2188,19 @@
       </c>
       <c r="F40">
         <f>F35/F37</f>
-        <v>0.39177625903780544</v>
+        <v>0.33403807596981594</v>
       </c>
       <c r="L40">
         <f>L35/L37</f>
-        <v>-0.23998795166491607</v>
+        <v>-0.22066912243195749</v>
       </c>
       <c r="R40">
         <f>R35/R37</f>
-        <v>0.16466714648504838</v>
+        <v>0.1721769890727684</v>
       </c>
       <c r="X40">
         <f>X35/X37</f>
-        <v>3.8967588820113634E-2</v>
+        <v>3.9076931194751668E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for giving real-time information to the forecast code
</commit_message>
<xml_diff>
--- a/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
+++ b/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\sam_dev\sam-analyses\2023\mirletz_laws_pvsc\sam_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7568238-3B3B-44EC-92C7-5ADF4C86565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAE0AF-6939-4C15-8DC1-E94195A1918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12360" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Method</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>Percent change due to energy</t>
+  </si>
+  <si>
+    <t>Price - patch</t>
+  </si>
+  <si>
+    <t>W/real time info</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Don't runn batt</t>
   </si>
 </sst>
 </file>
@@ -156,11 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -476,15 +484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3588BC-B3E7-4AEB-B5DC-1E4DB3FCD419}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,60 +508,108 @@
       <c r="E1">
         <v>8760</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8119098</v>
+        <v>8119090</v>
       </c>
       <c r="C2">
-        <v>8839129</v>
+        <v>8840408</v>
       </c>
       <c r="D2">
-        <v>8433096</v>
+        <v>8433026</v>
       </c>
       <c r="E2">
-        <v>8694613</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8518977</v>
+      </c>
+      <c r="F2">
+        <v>7639290</v>
+      </c>
+      <c r="G2">
+        <v>7980312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8045240</v>
+        <v>8045198</v>
       </c>
       <c r="C3">
-        <v>8487403</v>
+        <v>8731707</v>
       </c>
       <c r="D3">
-        <v>7398588</v>
+        <v>7739318</v>
       </c>
       <c r="E3">
-        <v>7618659</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7604898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>1-B3/B2</f>
-        <v>9.0968233170729551E-3</v>
+        <v>9.1010199418900539E-3</v>
       </c>
       <c r="C4">
         <f>1-C3/C2</f>
-        <v>3.9791929725202513E-2</v>
+        <v>1.2295925708406208E-2</v>
       </c>
       <c r="D4">
         <f>1-D3/D2</f>
-        <v>0.12267238508846579</v>
+        <v>8.2260863419607588E-2</v>
       </c>
       <c r="E4">
         <f>1-E3/E2</f>
-        <v>0.12374949868384022</v>
+        <v>0.10729915106003929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>8840408</v>
+      </c>
+      <c r="D7">
+        <v>8835871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>8484012</v>
+      </c>
+      <c r="D8">
+        <v>8731707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f>1-D8/D7</f>
+        <v>1.1788764231619009E-2</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E54FFCA-3A81-4895-A7A8-268220DEAC62}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
       <selection activeCell="W20" sqref="W20:X31"/>
     </sheetView>
   </sheetViews>
@@ -607,15 +663,15 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>6431.32</v>
+        <v>6429.19</v>
       </c>
       <c r="C3">
         <v>14576.3</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>6663.47</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>14576.3</v>
       </c>
       <c r="H3">
@@ -624,10 +680,10 @@
       <c r="I3">
         <v>14576.3</v>
       </c>
-      <c r="K3" s="3">
-        <v>9882.5</v>
-      </c>
-      <c r="L3" s="3">
+      <c r="K3">
+        <v>9344.69</v>
+      </c>
+      <c r="L3">
         <v>14576.3</v>
       </c>
       <c r="N3">
@@ -643,13 +699,13 @@
         <v>14576.3</v>
       </c>
       <c r="T3">
-        <v>4847.7299999999996</v>
+        <v>5097.43</v>
       </c>
       <c r="U3">
         <v>14576.3</v>
       </c>
       <c r="W3">
-        <v>14926.6</v>
+        <v>15048.5</v>
       </c>
       <c r="X3">
         <v>14576.3</v>
@@ -660,15 +716,15 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>7747.58</v>
+        <v>7747.6</v>
       </c>
       <c r="C4">
         <v>13895.1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>6492.63</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>13895.1</v>
       </c>
       <c r="H4">
@@ -677,10 +733,10 @@
       <c r="I4">
         <v>13895.1</v>
       </c>
-      <c r="K4" s="3">
-        <v>9398.2999999999993</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="K4">
+        <v>8754.26</v>
+      </c>
+      <c r="L4">
         <v>13895.1</v>
       </c>
       <c r="N4">
@@ -690,13 +746,13 @@
         <v>13895.1</v>
       </c>
       <c r="Q4">
-        <v>12515.4</v>
+        <v>9398.2999999999993</v>
       </c>
       <c r="R4">
         <v>13895.1</v>
       </c>
       <c r="T4">
-        <v>3757.32</v>
+        <v>4362.84</v>
       </c>
       <c r="U4">
         <v>13895.1</v>
@@ -717,15 +773,15 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>6845.01</v>
+        <v>6845</v>
       </c>
       <c r="C5">
         <v>14314.6</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>6631.32</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>14314.6</v>
       </c>
       <c r="H5">
@@ -734,32 +790,32 @@
       <c r="I5">
         <v>14314.6</v>
       </c>
-      <c r="K5" s="3">
-        <v>10699.5</v>
-      </c>
-      <c r="L5" s="3">
+      <c r="K5">
+        <v>9333.5300000000007</v>
+      </c>
+      <c r="L5">
         <v>14314.6</v>
       </c>
       <c r="N5">
-        <v>5903.77</v>
+        <v>5904.14</v>
       </c>
       <c r="O5">
         <v>14314.6</v>
       </c>
       <c r="Q5">
-        <v>14423.6</v>
+        <v>9851.23</v>
       </c>
       <c r="R5">
         <v>14314.6</v>
       </c>
       <c r="T5">
-        <v>4407.45</v>
+        <v>7631.07</v>
       </c>
       <c r="U5">
         <v>14314.6</v>
       </c>
       <c r="W5">
-        <v>14159.6</v>
+        <v>14307.5</v>
       </c>
       <c r="X5">
         <v>14314.6</v>
@@ -767,49 +823,49 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>6162.55</v>
+        <v>6162.58</v>
       </c>
       <c r="C6">
         <v>14556.4</v>
       </c>
-      <c r="E6" s="1">
-        <v>6550.82</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="E6">
+        <v>6550.77</v>
+      </c>
+      <c r="F6">
         <v>14556.4</v>
       </c>
       <c r="H6">
-        <v>9415.66</v>
+        <v>9415.76</v>
       </c>
       <c r="I6">
         <v>14556.4</v>
       </c>
-      <c r="K6" s="3">
-        <v>12516.2</v>
-      </c>
-      <c r="L6" s="3">
+      <c r="K6">
+        <v>9373.76</v>
+      </c>
+      <c r="L6">
         <v>14556.4</v>
       </c>
       <c r="N6">
-        <v>6075.52</v>
+        <v>6075.73</v>
       </c>
       <c r="O6">
         <v>14556.4</v>
       </c>
       <c r="Q6">
-        <v>12830</v>
+        <v>9770.43</v>
       </c>
       <c r="R6">
         <v>14556.4</v>
       </c>
       <c r="T6">
-        <v>4253.07</v>
+        <v>8593.2000000000007</v>
       </c>
       <c r="U6">
         <v>14556.4</v>
       </c>
       <c r="W6">
-        <v>15662.2</v>
+        <v>15559.9</v>
       </c>
       <c r="X6">
         <v>14556.4</v>
@@ -817,15 +873,15 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B7">
-        <v>7087.48</v>
+        <v>7087.63</v>
       </c>
       <c r="C7">
         <v>14459.1</v>
       </c>
-      <c r="E7" s="1">
-        <v>8229.9500000000007</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="E7">
+        <v>8231.18</v>
+      </c>
+      <c r="F7">
         <v>14459.1</v>
       </c>
       <c r="H7">
@@ -834,10 +890,10 @@
       <c r="I7">
         <v>14459.1</v>
       </c>
-      <c r="K7" s="3">
-        <v>11457.5</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="K7">
+        <v>9342.92</v>
+      </c>
+      <c r="L7">
         <v>14459.1</v>
       </c>
       <c r="N7">
@@ -847,19 +903,19 @@
         <v>14459.1</v>
       </c>
       <c r="Q7">
-        <v>11436.6</v>
+        <v>9284.4699999999993</v>
       </c>
       <c r="R7">
         <v>14459.1</v>
       </c>
       <c r="T7">
-        <v>4610.91</v>
+        <v>8629.48</v>
       </c>
       <c r="U7">
         <v>14459.1</v>
       </c>
       <c r="W7">
-        <v>13411.2</v>
+        <v>13650.3</v>
       </c>
       <c r="X7">
         <v>14459.1</v>
@@ -872,10 +928,10 @@
       <c r="C8">
         <v>14896.1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>12499.4</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>14896.1</v>
       </c>
       <c r="H8">
@@ -884,10 +940,10 @@
       <c r="I8">
         <v>14896.1</v>
       </c>
-      <c r="K8" s="3">
-        <v>18086.8</v>
-      </c>
-      <c r="L8" s="3">
+      <c r="K8">
+        <v>11366.7</v>
+      </c>
+      <c r="L8">
         <v>14896.1</v>
       </c>
       <c r="N8">
@@ -897,19 +953,19 @@
         <v>14896.1</v>
       </c>
       <c r="Q8">
-        <v>17966.3</v>
+        <v>13391</v>
       </c>
       <c r="R8">
         <v>14896.1</v>
       </c>
       <c r="T8">
-        <v>7376</v>
+        <v>7518.6</v>
       </c>
       <c r="U8">
         <v>14896.1</v>
       </c>
       <c r="W8">
-        <v>17702.3</v>
+        <v>17694.5</v>
       </c>
       <c r="X8">
         <v>14896.1</v>
@@ -917,15 +973,15 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B9">
-        <v>6871.79</v>
+        <v>6871.77</v>
       </c>
       <c r="C9">
         <v>14901.8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>7454.73</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>14901.8</v>
       </c>
       <c r="H9">
@@ -934,10 +990,10 @@
       <c r="I9">
         <v>14901.8</v>
       </c>
-      <c r="K9" s="3">
-        <v>15591.9</v>
-      </c>
-      <c r="L9" s="3">
+      <c r="K9">
+        <v>9454.5400000000009</v>
+      </c>
+      <c r="L9">
         <v>14901.8</v>
       </c>
       <c r="N9">
@@ -947,19 +1003,19 @@
         <v>14901.8</v>
       </c>
       <c r="Q9">
-        <v>11527.4</v>
+        <v>10693.6</v>
       </c>
       <c r="R9">
         <v>14901.8</v>
       </c>
       <c r="T9">
-        <v>5143.2</v>
+        <v>7852.35</v>
       </c>
       <c r="U9">
         <v>14901.8</v>
       </c>
       <c r="W9">
-        <v>15256.6</v>
+        <v>15520.6</v>
       </c>
       <c r="X9">
         <v>14901.8</v>
@@ -967,15 +1023,15 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B10">
-        <v>8014.91</v>
+        <v>8015.04</v>
       </c>
       <c r="C10">
         <v>15058.7</v>
       </c>
-      <c r="E10" s="1">
-        <v>9125.98</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="E10">
+        <v>9126</v>
+      </c>
+      <c r="F10">
         <v>15058.7</v>
       </c>
       <c r="H10">
@@ -984,32 +1040,32 @@
       <c r="I10">
         <v>15058.7</v>
       </c>
-      <c r="K10" s="3">
-        <v>18331.8</v>
-      </c>
-      <c r="L10" s="3">
+      <c r="K10">
+        <v>12150.6</v>
+      </c>
+      <c r="L10">
         <v>15058.7</v>
       </c>
       <c r="N10">
-        <v>7498.02</v>
+        <v>7498.71</v>
       </c>
       <c r="O10">
         <v>15058.7</v>
       </c>
       <c r="Q10">
-        <v>18456.400000000001</v>
+        <v>11856.8</v>
       </c>
       <c r="R10">
         <v>15058.7</v>
       </c>
       <c r="T10">
-        <v>6227.15</v>
+        <v>9329.2199999999993</v>
       </c>
       <c r="U10">
         <v>15058.7</v>
       </c>
       <c r="W10">
-        <v>18192.400000000001</v>
+        <v>18391.400000000001</v>
       </c>
       <c r="X10">
         <v>15058.7</v>
@@ -1017,15 +1073,15 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>7351.64</v>
+        <v>7351.66</v>
       </c>
       <c r="C11">
         <v>15203.5</v>
       </c>
-      <c r="E11" s="1">
-        <v>8900.27</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="E11">
+        <v>8901.0400000000009</v>
+      </c>
+      <c r="F11">
         <v>15203.5</v>
       </c>
       <c r="H11">
@@ -1034,10 +1090,10 @@
       <c r="I11">
         <v>15203.5</v>
       </c>
-      <c r="K11" s="3">
-        <v>15554.3</v>
-      </c>
-      <c r="L11" s="3">
+      <c r="K11">
+        <v>13019.8</v>
+      </c>
+      <c r="L11">
         <v>15203.5</v>
       </c>
       <c r="N11">
@@ -1047,19 +1103,19 @@
         <v>15203.5</v>
       </c>
       <c r="Q11">
-        <v>19063.599999999999</v>
+        <v>10408.6</v>
       </c>
       <c r="R11">
         <v>15203.5</v>
       </c>
       <c r="T11">
-        <v>6412.75</v>
+        <v>8244.3799999999992</v>
       </c>
       <c r="U11">
         <v>15203.5</v>
       </c>
       <c r="W11">
-        <v>16283</v>
+        <v>16547</v>
       </c>
       <c r="X11">
         <v>15203.5</v>
@@ -1067,15 +1123,15 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B12">
-        <v>8143.59</v>
+        <v>8143.58</v>
       </c>
       <c r="C12">
         <v>14877.2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>8836.15</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>14877.2</v>
       </c>
       <c r="H12">
@@ -1084,10 +1140,10 @@
       <c r="I12">
         <v>14877.2</v>
       </c>
-      <c r="K12" s="3">
-        <v>18336.599999999999</v>
-      </c>
-      <c r="L12" s="3">
+      <c r="K12">
+        <v>12467.2</v>
+      </c>
+      <c r="L12">
         <v>14877.2</v>
       </c>
       <c r="N12">
@@ -1097,19 +1153,19 @@
         <v>14877.2</v>
       </c>
       <c r="Q12">
-        <v>19066.8</v>
+        <v>12956.4</v>
       </c>
       <c r="R12">
         <v>14877.2</v>
       </c>
       <c r="T12">
-        <v>6621.5</v>
+        <v>8224.51</v>
       </c>
       <c r="U12">
         <v>14877.2</v>
       </c>
       <c r="W12">
-        <v>16891.400000000001</v>
+        <v>17136.3</v>
       </c>
       <c r="X12">
         <v>14877.2</v>
@@ -1117,15 +1173,15 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B13">
-        <v>9282.35</v>
+        <v>9282.02</v>
       </c>
       <c r="C13">
         <v>14976.4</v>
       </c>
-      <c r="E13" s="1">
-        <v>10476</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="E13">
+        <v>10476.1</v>
+      </c>
+      <c r="F13">
         <v>14976.4</v>
       </c>
       <c r="H13">
@@ -1134,10 +1190,10 @@
       <c r="I13">
         <v>14976.4</v>
       </c>
-      <c r="K13" s="3">
-        <v>17541.599999999999</v>
-      </c>
-      <c r="L13" s="3">
+      <c r="K13">
+        <v>11447.3</v>
+      </c>
+      <c r="L13">
         <v>14976.4</v>
       </c>
       <c r="N13">
@@ -1147,19 +1203,19 @@
         <v>14976.4</v>
       </c>
       <c r="Q13">
-        <v>17654</v>
+        <v>12538.1</v>
       </c>
       <c r="R13">
         <v>14976.4</v>
       </c>
       <c r="T13">
-        <v>6576.02</v>
+        <v>7258.35</v>
       </c>
       <c r="U13">
         <v>14976.4</v>
       </c>
       <c r="W13">
-        <v>17390</v>
+        <v>17654</v>
       </c>
       <c r="X13">
         <v>14976.4</v>
@@ -1167,15 +1223,15 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B14">
-        <v>6540.57</v>
+        <v>6540.54</v>
       </c>
       <c r="C14">
         <v>14456.5</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>6584.05</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>14456.5</v>
       </c>
       <c r="H14">
@@ -1184,10 +1240,10 @@
       <c r="I14">
         <v>14456.5</v>
       </c>
-      <c r="K14" s="3">
-        <v>10518.1</v>
-      </c>
-      <c r="L14" s="3">
+      <c r="K14">
+        <v>9334.4500000000007</v>
+      </c>
+      <c r="L14">
         <v>14456.5</v>
       </c>
       <c r="N14">
@@ -1197,19 +1253,19 @@
         <v>14456.5</v>
       </c>
       <c r="Q14">
-        <v>14062.1</v>
+        <v>10993.4</v>
       </c>
       <c r="R14">
         <v>14456.5</v>
       </c>
       <c r="T14">
-        <v>5365.53</v>
+        <v>6751.55</v>
       </c>
       <c r="U14">
         <v>14456.5</v>
       </c>
       <c r="W14">
-        <v>14188.9</v>
+        <v>14372.3</v>
       </c>
       <c r="X14">
         <v>14456.5</v>
@@ -1221,7 +1277,7 @@
       </c>
       <c r="B16">
         <f>SUM(B3:B14)</f>
-        <v>90399.91</v>
+        <v>90397.73</v>
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
@@ -1229,7 +1285,7 @@
       </c>
       <c r="E16">
         <f>SUM(E3:E14)</f>
-        <v>98444.77</v>
+        <v>98446.840000000011</v>
       </c>
       <c r="F16">
         <f>SUM(F3:F14)</f>
@@ -1237,7 +1293,7 @@
       </c>
       <c r="H16">
         <f>SUM(H3:H14)</f>
-        <v>120100.98999999999</v>
+        <v>120101.09</v>
       </c>
       <c r="I16">
         <f>SUM(I3:I14)</f>
@@ -1245,7 +1301,7 @@
       </c>
       <c r="K16">
         <f>SUM(K3:K14)</f>
-        <v>167915.1</v>
+        <v>125389.75</v>
       </c>
       <c r="L16">
         <f>SUM(L3:L14)</f>
@@ -1253,7 +1309,7 @@
       </c>
       <c r="N16">
         <f>SUM(N3:N14)</f>
-        <v>81285.17</v>
+        <v>81286.440000000017</v>
       </c>
       <c r="O16">
         <f>SUM(O3:O14)</f>
@@ -1261,7 +1317,7 @@
       </c>
       <c r="Q16">
         <f>SUM(Q3:Q14)</f>
-        <v>178884.69999999998</v>
+        <v>131024.83</v>
       </c>
       <c r="R16">
         <f>SUM(R3:R14)</f>
@@ -1269,7 +1325,7 @@
       </c>
       <c r="T16">
         <f>SUM(T3:T14)</f>
-        <v>65598.63</v>
+        <v>89492.98000000001</v>
       </c>
       <c r="U16">
         <f>SUM(U3:U14)</f>
@@ -1277,7 +1333,7 @@
       </c>
       <c r="W16">
         <f>SUM(W3:W14)</f>
-        <v>189798.1</v>
+        <v>191616.19999999998</v>
       </c>
       <c r="X16">
         <f>SUM(X3:X14)</f>
@@ -1290,35 +1346,35 @@
       </c>
       <c r="C17">
         <f>C16-B16</f>
-        <v>85771.790000000008</v>
+        <v>85773.970000000016</v>
       </c>
       <c r="F17">
         <f>F16-E16</f>
-        <v>77726.930000000008</v>
+        <v>77724.86</v>
       </c>
       <c r="I17">
         <f>I16-H16</f>
-        <v>56070.710000000021</v>
+        <v>56070.610000000015</v>
       </c>
       <c r="L17">
         <f>L16-K16</f>
-        <v>8256.6000000000058</v>
+        <v>50781.950000000012</v>
       </c>
       <c r="O17">
         <f>O16-N16</f>
-        <v>94886.530000000013</v>
+        <v>94885.26</v>
       </c>
       <c r="R17">
         <f>R16-Q16</f>
-        <v>-2712.9999999999709</v>
+        <v>45146.87000000001</v>
       </c>
       <c r="U17">
         <f>U16-T16</f>
-        <v>110573.07</v>
+        <v>86678.720000000001</v>
       </c>
       <c r="X17">
         <f>X16-W16</f>
-        <v>-13626.399999999994</v>
+        <v>-15444.499999999971</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
@@ -1327,35 +1383,35 @@
       </c>
       <c r="F18">
         <f>C17-F17</f>
-        <v>8044.8600000000006</v>
+        <v>8049.1100000000151</v>
       </c>
       <c r="G18">
         <f>1-F17/C17</f>
-        <v>9.3793775319367834E-2</v>
+        <v>9.3840940322571176E-2</v>
       </c>
       <c r="L18">
         <f>I17-L17</f>
-        <v>47814.110000000015</v>
+        <v>5288.6600000000035</v>
       </c>
       <c r="M18">
         <f>1-L17/I17</f>
-        <v>0.85274664793793398</v>
+        <v>9.432142792810716E-2</v>
       </c>
       <c r="R18">
         <f>O17-R17</f>
-        <v>97599.529999999984</v>
+        <v>49738.389999999985</v>
       </c>
       <c r="S18">
         <f>1-R17/O17</f>
-        <v>1.0285920456781377</v>
+        <v>0.52419511734488566</v>
       </c>
       <c r="X18">
         <f>U17-X17</f>
-        <v>124199.47</v>
+        <v>102123.21999999997</v>
       </c>
       <c r="Y18">
         <f>1-X17/U17</f>
-        <v>1.1232343463015</v>
+        <v>1.1781809883671559</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
@@ -1365,49 +1421,49 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>24850.1</v>
+        <v>24847.3</v>
       </c>
       <c r="C20">
         <v>136681</v>
       </c>
-      <c r="E20" s="2">
-        <v>25530</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="E20">
+        <v>25529.599999999999</v>
+      </c>
+      <c r="F20">
         <v>136681</v>
       </c>
       <c r="H20">
-        <v>13936.5</v>
+        <v>13973.8</v>
       </c>
       <c r="I20">
         <v>136681</v>
       </c>
-      <c r="K20" s="4">
-        <v>13577.5</v>
-      </c>
-      <c r="L20" s="4">
+      <c r="K20">
+        <v>14955.8</v>
+      </c>
+      <c r="L20">
         <v>136681</v>
       </c>
       <c r="N20">
-        <v>22626.3</v>
+        <v>22626.2</v>
       </c>
       <c r="O20">
         <v>136681</v>
       </c>
       <c r="Q20">
-        <v>23260.400000000001</v>
+        <v>24993.5</v>
       </c>
       <c r="R20">
         <v>136681</v>
       </c>
       <c r="T20">
-        <v>19961.400000000001</v>
+        <v>19780.8</v>
       </c>
       <c r="U20">
         <v>136681</v>
       </c>
       <c r="W20">
-        <v>21047.7</v>
+        <v>20941.099999999999</v>
       </c>
       <c r="X20">
         <v>136681</v>
@@ -1415,49 +1471,49 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>16698.2</v>
+        <v>16697.900000000001</v>
       </c>
       <c r="C21">
         <v>119047</v>
       </c>
-      <c r="E21" s="2">
-        <v>17915.599999999999</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="E21">
+        <v>17915.2</v>
+      </c>
+      <c r="F21">
         <v>119047</v>
       </c>
       <c r="H21">
-        <v>7732.89</v>
+        <v>7713.95</v>
       </c>
       <c r="I21">
         <v>119047</v>
       </c>
-      <c r="K21" s="4">
-        <v>8047.9</v>
-      </c>
-      <c r="L21" s="4">
+      <c r="K21">
+        <v>9381.0400000000009</v>
+      </c>
+      <c r="L21">
         <v>119047</v>
       </c>
       <c r="N21">
-        <v>14141.4</v>
+        <v>14141.1</v>
       </c>
       <c r="O21">
         <v>119047</v>
       </c>
       <c r="Q21">
-        <v>16152.8</v>
+        <v>17380.7</v>
       </c>
       <c r="R21">
         <v>119047</v>
       </c>
       <c r="T21">
-        <v>9345.9</v>
+        <v>8940.85</v>
       </c>
       <c r="U21">
         <v>119047</v>
       </c>
       <c r="W21">
-        <v>13590.9</v>
+        <v>13462.9</v>
       </c>
       <c r="X21">
         <v>119047</v>
@@ -1465,49 +1521,49 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22">
-        <v>25580.400000000001</v>
+        <v>25581.1</v>
       </c>
       <c r="C22">
         <v>135863</v>
       </c>
-      <c r="E22" s="2">
-        <v>26628.400000000001</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="E22">
+        <v>26629.200000000001</v>
+      </c>
+      <c r="F22">
         <v>135863</v>
       </c>
       <c r="H22">
-        <v>15528.9</v>
+        <v>15466</v>
       </c>
       <c r="I22">
         <v>135863</v>
       </c>
-      <c r="K22" s="4">
-        <v>14356.9</v>
-      </c>
-      <c r="L22" s="4">
+      <c r="K22">
+        <v>16305.1</v>
+      </c>
+      <c r="L22">
         <v>135863</v>
       </c>
       <c r="N22">
-        <v>23248.799999999999</v>
+        <v>23249.9</v>
       </c>
       <c r="O22">
         <v>135863</v>
       </c>
       <c r="Q22">
-        <v>26074.799999999999</v>
+        <v>26846.9</v>
       </c>
       <c r="R22">
         <v>135863</v>
       </c>
       <c r="T22">
-        <v>19335.3</v>
+        <v>19261.400000000001</v>
       </c>
       <c r="U22">
         <v>135863</v>
       </c>
       <c r="W22">
-        <v>21761</v>
+        <v>21578.799999999999</v>
       </c>
       <c r="X22">
         <v>135863</v>
@@ -1515,49 +1571,49 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>17723.8</v>
+        <v>17724.900000000001</v>
       </c>
       <c r="C23">
         <v>132398</v>
       </c>
-      <c r="E23" s="2">
-        <v>18477.5</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="E23">
+        <v>18478.5</v>
+      </c>
+      <c r="F23">
         <v>132398</v>
       </c>
       <c r="H23">
-        <v>8274.39</v>
+        <v>8250.44</v>
       </c>
       <c r="I23">
         <v>132398</v>
       </c>
-      <c r="K23" s="4">
-        <v>8076.78</v>
-      </c>
-      <c r="L23" s="4">
+      <c r="K23">
+        <v>8306.2199999999993</v>
+      </c>
+      <c r="L23">
         <v>132398</v>
       </c>
       <c r="N23">
-        <v>15011.6</v>
+        <v>15013.2</v>
       </c>
       <c r="O23">
         <v>132398</v>
       </c>
       <c r="Q23">
-        <v>17479.099999999999</v>
+        <v>18046.8</v>
       </c>
       <c r="R23">
         <v>132398</v>
       </c>
       <c r="T23">
-        <v>11767.7</v>
+        <v>11669.7</v>
       </c>
       <c r="U23">
         <v>132398</v>
       </c>
       <c r="W23">
-        <v>14763</v>
+        <v>14687.6</v>
       </c>
       <c r="X23">
         <v>132398</v>
@@ -1565,49 +1621,49 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B24">
-        <v>28336.6</v>
+        <v>28337.599999999999</v>
       </c>
       <c r="C24">
         <v>139577</v>
       </c>
-      <c r="E24" s="2">
-        <v>28433.1</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="E24">
+        <v>28434.1</v>
+      </c>
+      <c r="F24">
         <v>139577</v>
       </c>
       <c r="H24">
-        <v>16828.900000000001</v>
+        <v>16780.7</v>
       </c>
       <c r="I24">
         <v>139577</v>
       </c>
-      <c r="K24" s="4">
-        <v>16958.599999999999</v>
-      </c>
-      <c r="L24" s="4">
+      <c r="K24">
+        <v>17611.599999999999</v>
+      </c>
+      <c r="L24">
         <v>139577</v>
       </c>
       <c r="N24">
-        <v>25950.6</v>
+        <v>25952.1</v>
       </c>
       <c r="O24">
         <v>139577</v>
       </c>
       <c r="Q24">
-        <v>28625.4</v>
+        <v>28874.2</v>
       </c>
       <c r="R24">
         <v>139577</v>
       </c>
       <c r="T24">
-        <v>23066.1</v>
+        <v>22995</v>
       </c>
       <c r="U24">
         <v>139577</v>
       </c>
       <c r="W24">
-        <v>25093.7</v>
+        <v>25045</v>
       </c>
       <c r="X24">
         <v>139577</v>
@@ -1615,49 +1671,49 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B25">
-        <v>28673.1</v>
+        <v>28673.8</v>
       </c>
       <c r="C25">
         <v>140124</v>
       </c>
-      <c r="E25" s="2">
-        <v>29350.400000000001</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="E25">
+        <v>29351.1</v>
+      </c>
+      <c r="F25">
         <v>140124</v>
       </c>
       <c r="H25">
-        <v>18325</v>
+        <v>18323.3</v>
       </c>
       <c r="I25">
         <v>140124</v>
       </c>
-      <c r="K25" s="4">
-        <v>18367.400000000001</v>
-      </c>
-      <c r="L25" s="4">
+      <c r="K25">
+        <v>18471.5</v>
+      </c>
+      <c r="L25">
         <v>140124</v>
       </c>
       <c r="N25">
-        <v>26243.7</v>
+        <v>26244.9</v>
       </c>
       <c r="O25">
         <v>140124</v>
       </c>
       <c r="Q25">
-        <v>28632.9</v>
+        <v>29429.200000000001</v>
       </c>
       <c r="R25">
         <v>140124</v>
       </c>
       <c r="T25">
-        <v>29055.5</v>
+        <v>29151</v>
       </c>
       <c r="U25">
         <v>140124</v>
       </c>
       <c r="W25">
-        <v>25187.200000000001</v>
+        <v>25122.7</v>
       </c>
       <c r="X25">
         <v>140124</v>
@@ -1665,49 +1721,49 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>28617.5</v>
+        <v>28617.599999999999</v>
       </c>
       <c r="C26">
         <v>142832</v>
       </c>
-      <c r="E26" s="2">
-        <v>28917.3</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="E26">
+        <v>28917.5</v>
+      </c>
+      <c r="F26">
         <v>142832</v>
       </c>
       <c r="H26">
-        <v>19766</v>
+        <v>19771.3</v>
       </c>
       <c r="I26">
         <v>142832</v>
       </c>
-      <c r="K26" s="4">
-        <v>18874.7</v>
-      </c>
-      <c r="L26" s="4">
+      <c r="K26">
+        <v>20802.8</v>
+      </c>
+      <c r="L26">
         <v>142832</v>
       </c>
       <c r="N26">
-        <v>24778.5</v>
+        <v>24779.200000000001</v>
       </c>
       <c r="O26">
         <v>142832</v>
       </c>
       <c r="Q26">
-        <v>28250.9</v>
+        <v>28878.3</v>
       </c>
       <c r="R26">
         <v>142832</v>
       </c>
       <c r="T26">
-        <v>24069.3</v>
+        <v>23907.3</v>
       </c>
       <c r="U26">
         <v>142832</v>
       </c>
       <c r="W26">
-        <v>26357.1</v>
+        <v>26301.9</v>
       </c>
       <c r="X26">
         <v>142832</v>
@@ -1715,49 +1771,49 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>31599.200000000001</v>
+        <v>31599.7</v>
       </c>
       <c r="C27">
         <v>147121</v>
       </c>
-      <c r="E27" s="2">
-        <v>31931.3</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="E27">
+        <v>31932.1</v>
+      </c>
+      <c r="F27">
         <v>147121</v>
       </c>
       <c r="H27">
-        <v>20738.599999999999</v>
+        <v>20873.5</v>
       </c>
       <c r="I27">
         <v>147121</v>
       </c>
-      <c r="K27" s="4">
-        <v>20419.3</v>
-      </c>
-      <c r="L27" s="4">
+      <c r="K27">
+        <v>21825.4</v>
+      </c>
+      <c r="L27">
         <v>147121</v>
       </c>
       <c r="N27">
-        <v>28747.200000000001</v>
+        <v>28748.3</v>
       </c>
       <c r="O27">
         <v>147121</v>
       </c>
       <c r="Q27">
-        <v>31078.2</v>
+        <v>32364.9</v>
       </c>
       <c r="R27">
         <v>147121</v>
       </c>
       <c r="T27">
-        <v>28837</v>
+        <v>28895.4</v>
       </c>
       <c r="U27">
         <v>147121</v>
       </c>
       <c r="W27">
-        <v>28273.4</v>
+        <v>28157.4</v>
       </c>
       <c r="X27">
         <v>147121</v>
@@ -1770,44 +1826,44 @@
       <c r="C28">
         <v>140368</v>
       </c>
-      <c r="E28" s="2">
-        <v>28739.9</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="E28">
+        <v>28739.8</v>
+      </c>
+      <c r="F28">
         <v>140368</v>
       </c>
       <c r="H28">
-        <v>18376.8</v>
+        <v>18377.3</v>
       </c>
       <c r="I28">
         <v>140368</v>
       </c>
-      <c r="K28" s="4">
-        <v>18131.8</v>
-      </c>
-      <c r="L28" s="4">
+      <c r="K28">
+        <v>19716.099999999999</v>
+      </c>
+      <c r="L28">
         <v>140368</v>
       </c>
       <c r="N28">
-        <v>26907.1</v>
+        <v>26907.3</v>
       </c>
       <c r="O28">
         <v>140368</v>
       </c>
       <c r="Q28">
-        <v>28152.2</v>
+        <v>29077.3</v>
       </c>
       <c r="R28">
         <v>140368</v>
       </c>
       <c r="T28">
-        <v>24798.799999999999</v>
+        <v>24774.3</v>
       </c>
       <c r="U28">
         <v>140368</v>
       </c>
       <c r="W28">
-        <v>24842.2</v>
+        <v>24931.3</v>
       </c>
       <c r="X28">
         <v>140368</v>
@@ -1815,49 +1871,49 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29">
-        <v>32493.8</v>
+        <v>32494</v>
       </c>
       <c r="C29">
         <v>142469</v>
       </c>
-      <c r="E29" s="2">
-        <v>31415.7</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="E29">
+        <v>31415.9</v>
+      </c>
+      <c r="F29">
         <v>142469</v>
       </c>
       <c r="H29">
-        <v>22316.9</v>
+        <v>22328.3</v>
       </c>
       <c r="I29">
         <v>142469</v>
       </c>
-      <c r="K29" s="4">
-        <v>20289.7</v>
-      </c>
-      <c r="L29" s="4">
+      <c r="K29">
+        <v>22718</v>
+      </c>
+      <c r="L29">
         <v>142469</v>
       </c>
       <c r="N29">
-        <v>30286.2</v>
+        <v>30286.5</v>
       </c>
       <c r="O29">
         <v>142469</v>
       </c>
       <c r="Q29">
-        <v>30938.3</v>
+        <v>31437</v>
       </c>
       <c r="R29">
         <v>142469</v>
       </c>
       <c r="T29">
-        <v>31694.5</v>
+        <v>31764.6</v>
       </c>
       <c r="U29">
         <v>142469</v>
       </c>
       <c r="W29">
-        <v>28450.2</v>
+        <v>28423.1</v>
       </c>
       <c r="X29">
         <v>142469</v>
@@ -1865,49 +1921,49 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30">
-        <v>26037</v>
+        <v>26038.400000000001</v>
       </c>
       <c r="C30">
         <v>137239</v>
       </c>
-      <c r="E30" s="2">
-        <v>26037.5</v>
-      </c>
-      <c r="F30" s="2">
+      <c r="E30">
+        <v>26038.9</v>
+      </c>
+      <c r="F30">
         <v>137239</v>
       </c>
       <c r="H30">
-        <v>16073.6</v>
+        <v>16083.2</v>
       </c>
       <c r="I30">
         <v>137239</v>
       </c>
-      <c r="K30" s="4">
-        <v>13720.5</v>
-      </c>
-      <c r="L30" s="4">
+      <c r="K30">
+        <v>15430.5</v>
+      </c>
+      <c r="L30">
         <v>137239</v>
       </c>
       <c r="N30">
-        <v>24212.7</v>
+        <v>24214.5</v>
       </c>
       <c r="O30">
         <v>137239</v>
       </c>
       <c r="Q30">
-        <v>24002.1</v>
+        <v>24925</v>
       </c>
       <c r="R30">
         <v>137239</v>
       </c>
       <c r="T30">
-        <v>24749.200000000001</v>
+        <v>24793.5</v>
       </c>
       <c r="U30">
         <v>137239</v>
       </c>
       <c r="W30">
-        <v>22464.9</v>
+        <v>22505.200000000001</v>
       </c>
       <c r="X30">
         <v>137239</v>
@@ -1915,49 +1971,49 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B31">
-        <v>24918.7</v>
+        <v>24918.400000000001</v>
       </c>
       <c r="C31">
         <v>135534</v>
       </c>
-      <c r="E31" s="2">
-        <v>24975</v>
-      </c>
-      <c r="F31" s="2">
+      <c r="E31">
+        <v>24974.799999999999</v>
+      </c>
+      <c r="F31">
         <v>135534</v>
       </c>
       <c r="H31">
-        <v>14582</v>
+        <v>14540.3</v>
       </c>
       <c r="I31">
         <v>135534</v>
       </c>
-      <c r="K31" s="4">
-        <v>13015.7</v>
-      </c>
-      <c r="L31" s="4">
+      <c r="K31">
+        <v>14070.3</v>
+      </c>
+      <c r="L31">
         <v>135534</v>
       </c>
       <c r="N31">
-        <v>23179.1</v>
+        <v>23179.8</v>
       </c>
       <c r="O31">
         <v>135534</v>
       </c>
       <c r="Q31">
-        <v>22985.599999999999</v>
+        <v>24352.3</v>
       </c>
       <c r="R31">
         <v>135534</v>
       </c>
       <c r="T31">
-        <v>19926</v>
+        <v>19946.099999999999</v>
       </c>
       <c r="U31">
         <v>135534</v>
       </c>
       <c r="W31">
-        <v>19826.099999999999</v>
+        <v>19815.900000000001</v>
       </c>
       <c r="X31">
         <v>135534</v>
@@ -1966,7 +2022,7 @@
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B33">
         <f>SUM(B20:B31)</f>
-        <v>314316.50000000006</v>
+        <v>314318.80000000005</v>
       </c>
       <c r="C33">
         <f>SUM(C20:C31)</f>
@@ -1974,7 +2030,7 @@
       </c>
       <c r="E33">
         <f>SUM(E20:E31)</f>
-        <v>318351.69999999995</v>
+        <v>318356.7</v>
       </c>
       <c r="F33">
         <f>SUM(F20:F31)</f>
@@ -1982,7 +2038,7 @@
       </c>
       <c r="H33">
         <f>SUM(H20:H31)</f>
-        <v>192480.47999999998</v>
+        <v>192482.09</v>
       </c>
       <c r="I33">
         <f>SUM(I20:I31)</f>
@@ -1990,7 +2046,7 @@
       </c>
       <c r="K33">
         <f>SUM(K20:K31)</f>
-        <v>183836.78000000003</v>
+        <v>199594.36000000002</v>
       </c>
       <c r="L33">
         <f>SUM(L20:L31)</f>
@@ -1998,7 +2054,7 @@
       </c>
       <c r="N33">
         <f>SUM(N20:N31)</f>
-        <v>285333.2</v>
+        <v>285342.99999999994</v>
       </c>
       <c r="O33">
         <f>SUM(O20:O31)</f>
@@ -2006,7 +2062,7 @@
       </c>
       <c r="Q33">
         <f>SUM(Q20:Q31)</f>
-        <v>305632.69999999995</v>
+        <v>316606.09999999998</v>
       </c>
       <c r="R33">
         <f>SUM(R20:R31)</f>
@@ -2014,7 +2070,7 @@
       </c>
       <c r="T33">
         <f>SUM(T20:T31)</f>
-        <v>266606.69999999995</v>
+        <v>265879.94999999995</v>
       </c>
       <c r="U33">
         <f>SUM(U20:U31)</f>
@@ -2022,7 +2078,7 @@
       </c>
       <c r="W33">
         <f>SUM(W20:W31)</f>
-        <v>271657.40000000002</v>
+        <v>270972.90000000002</v>
       </c>
       <c r="X33">
         <f>SUM(X20:X31)</f>
@@ -2035,51 +2091,51 @@
       </c>
       <c r="C34">
         <f>C33-B33</f>
-        <v>1334936.5</v>
+        <v>1334934.2</v>
       </c>
       <c r="F34">
         <f>F33-E33</f>
-        <v>1330901.3</v>
+        <v>1330896.3</v>
       </c>
       <c r="G34">
         <f>1-F34/C34</f>
-        <v>3.0227655023290501E-3</v>
+        <v>3.0247932819459367E-3</v>
       </c>
       <c r="I34">
         <f>I33-H33</f>
-        <v>1456772.52</v>
+        <v>1456770.91</v>
       </c>
       <c r="L34">
         <f>L33-K33</f>
-        <v>1465416.22</v>
+        <v>1449658.64</v>
       </c>
       <c r="M34">
         <f>1-L34/I34</f>
-        <v>-5.9334589864448173E-3</v>
+        <v>4.8822158317261E-3</v>
       </c>
       <c r="O34">
         <f>O33-N33</f>
-        <v>1363919.8</v>
+        <v>1363910</v>
       </c>
       <c r="R34">
         <f>R33-Q33</f>
-        <v>1343620.3</v>
+        <v>1332646.8999999999</v>
       </c>
       <c r="S34">
         <f>1-R34/O34</f>
-        <v>1.4883206475923338E-2</v>
+        <v>2.2921673717474111E-2</v>
       </c>
       <c r="U34">
         <f>U33-T33</f>
-        <v>1382646.3</v>
+        <v>1383373.05</v>
       </c>
       <c r="X34">
         <f>X33-W33</f>
-        <v>1377595.6</v>
+        <v>1378280.1</v>
       </c>
       <c r="Y34">
         <f>1-X34/U34</f>
-        <v>3.6529226599745224E-3</v>
+        <v>3.6815449021505575E-3</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
@@ -2088,19 +2144,19 @@
       </c>
       <c r="F35">
         <f>C34-F34</f>
-        <v>4035.1999999999534</v>
+        <v>4037.8999999999069</v>
       </c>
       <c r="L35">
         <f>I34-L34</f>
-        <v>-8643.6999999999534</v>
+        <v>7112.2700000000186</v>
       </c>
       <c r="R35">
         <f>O34-R34</f>
-        <v>20299.5</v>
+        <v>31263.100000000093</v>
       </c>
       <c r="X35">
         <f>U34-X34</f>
-        <v>5050.6999999999534</v>
+        <v>5092.9499999999534</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
@@ -2109,35 +2165,35 @@
       </c>
       <c r="C36">
         <f>C17+C34</f>
-        <v>1420708.29</v>
+        <v>1420708.17</v>
       </c>
       <c r="F36">
         <f>F17+F34</f>
-        <v>1408628.23</v>
+        <v>1408621.1600000001</v>
       </c>
       <c r="I36">
         <f>I17+I34</f>
-        <v>1512843.23</v>
+        <v>1512841.52</v>
       </c>
       <c r="L36">
         <f>L17+L34</f>
-        <v>1473672.82</v>
+        <v>1500440.5899999999</v>
       </c>
       <c r="O36">
         <f>O17+O34</f>
-        <v>1458806.33</v>
+        <v>1458795.26</v>
       </c>
       <c r="R36">
         <f>R17+R34</f>
-        <v>1340907.3</v>
+        <v>1377793.77</v>
       </c>
       <c r="U36">
         <f>U17+U34</f>
-        <v>1493219.37</v>
+        <v>1470051.77</v>
       </c>
       <c r="X36">
         <f>X17+X34</f>
-        <v>1363969.2000000002</v>
+        <v>1362835.6</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
@@ -2146,19 +2202,19 @@
       </c>
       <c r="F37">
         <f>C36-F36</f>
-        <v>12080.060000000056</v>
+        <v>12087.009999999776</v>
       </c>
       <c r="L37">
         <f>I36-L36</f>
-        <v>39170.409999999916</v>
+        <v>12400.930000000168</v>
       </c>
       <c r="R37">
         <f>O36-R36</f>
-        <v>117899.03000000003</v>
+        <v>81001.489999999991</v>
       </c>
       <c r="X37">
         <f>U36-X36</f>
-        <v>129250.16999999993</v>
+        <v>107216.16999999993</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
@@ -2167,19 +2223,19 @@
       </c>
       <c r="F39">
         <f>F18/F37</f>
-        <v>0.66596192403017562</v>
+        <v>0.66593061476743742</v>
       </c>
       <c r="L39">
         <f>L18/L37</f>
-        <v>1.2206691224319612</v>
+        <v>0.42647285324567852</v>
       </c>
       <c r="R39">
         <f>R18/R37</f>
-        <v>0.82782301092723121</v>
+        <v>0.61404290217377466</v>
       </c>
       <c r="X39">
         <f>X18/X37</f>
-        <v>0.96092306880524858</v>
+        <v>0.95249830319437867</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
@@ -2188,19 +2244,19 @@
       </c>
       <c r="F40">
         <f>F35/F37</f>
-        <v>0.33403807596981594</v>
+        <v>0.33406938523257462</v>
       </c>
       <c r="L40">
         <f>L35/L37</f>
-        <v>-0.22066912243195749</v>
+        <v>0.57352714675430971</v>
       </c>
       <c r="R40">
         <f>R35/R37</f>
-        <v>0.1721769890727684</v>
+        <v>0.38595709782622639</v>
       </c>
       <c r="X40">
         <f>X35/X37</f>
-        <v>3.9076931194751668E-2</v>
+        <v>4.7501696805621364E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove unused files, update final number crunching sheet
</commit_message>
<xml_diff>
--- a/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
+++ b/2023/mirletz_laws_pvsc/sam_results/number_crunching.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\sam_dev\sam-analyses\2023\mirletz_laws_pvsc\sam_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAE0AF-6939-4C15-8DC1-E94195A1918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DC675C-C414-439F-A252-47284A3B26AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
+    <workbookView xWindow="34125" yWindow="3390" windowWidth="17280" windowHeight="8970" xr2:uid="{2DA5AA17-C658-4D07-AA75-E70A6B71FE12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3588BC-B3E7-4AEB-B5DC-1E4DB3FCD419}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,6 +576,12 @@
         <v>0.10729915106003929</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f>D2*0.08</f>
+        <v>674642.08</v>
+      </c>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>28</v>
@@ -604,6 +610,10 @@
       </c>
       <c r="D8">
         <v>8731707</v>
+      </c>
+      <c r="F8">
+        <f>D8/C8</f>
+        <v>1.0291955032595428</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -621,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E54FFCA-3A81-4895-A7A8-268220DEAC62}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20:X31"/>
+    <sheetView topLeftCell="I8" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>